<commit_message>
First commit i 2 years. Total makeover with new regobs api and python 3.
</commit_message>
<xml_diff>
--- a/varsomdata/input/matrixconfiguration.v2.xlsx
+++ b/varsomdata/input/matrixconfiguration.v2.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ragnarekker/Dropbox/Kode/Python/varsomdata/varsomdata/input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="38180" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -52,22 +60,10 @@
     <t>label_trigger</t>
   </si>
   <si>
-    <t>1 - Harmloest</t>
-  </si>
-  <si>
-    <t>2 - Smaa</t>
-  </si>
-  <si>
     <t>3 - Middels</t>
   </si>
   <si>
-    <t>5 - Svaert store</t>
-  </si>
-  <si>
     <t>4 - Store</t>
-  </si>
-  <si>
-    <t>Naturlig utloest</t>
   </si>
   <si>
     <t>Sannsynlig, Meget sannsynlig</t>
@@ -89,9 +85,6 @@
   </si>
   <si>
     <t>Noen bratte heng</t>
-  </si>
-  <si>
-    <t>Isolerte faresoner</t>
   </si>
   <si>
     <t>data_set</t>
@@ -145,9 +138,6 @@
     <t>Most</t>
   </si>
   <si>
-    <t>De fleste bratte heng, Ogsaa i mindre bratt terreng</t>
-  </si>
-  <si>
     <t>Mange bratte heng</t>
   </si>
   <si>
@@ -173,6 +163,24 @@
   </si>
   <si>
     <t>recomended_danger_level</t>
+  </si>
+  <si>
+    <t>Naturlig utløst</t>
+  </si>
+  <si>
+    <t>2 - Små</t>
+  </si>
+  <si>
+    <t>5 - Svært store</t>
+  </si>
+  <si>
+    <t>De fleste bratte heng, Også i mindre bratt terreng</t>
+  </si>
+  <si>
+    <t>1 - Harmløst (sluff)</t>
+  </si>
+  <si>
+    <t>Få bratte heng</t>
   </si>
 </sst>
 </file>
@@ -279,9 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="200">
+  <cellStyleXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -550,107 +560,108 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="200">
+  <cellStyles count="202">
+    <cellStyle name="Benyttet hyperkobling" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="199" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="6" builtinId="8" hidden="1"/>
@@ -750,6 +761,7 @@
     <cellStyle name="Hyperkobling" xfId="194" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="196" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1090,10 +1102,10 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="21" customWidth="1"/>
@@ -1110,7 +1122,7 @@
     <col min="13" max="16384" width="10.83203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1" ht="16">
+    <row r="1" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1142,16 +1154,16 @@
         <v>8</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B2" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -1163,7 +1175,7 @@
       </c>
       <c r="D2" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E2" s="22">
         <v>100</v>
@@ -1196,10 +1208,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B3" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -1211,7 +1223,7 @@
       </c>
       <c r="D3" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E3" s="22">
         <v>200</v>
@@ -1244,14 +1256,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B4" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C4" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -1259,7 +1271,7 @@
       </c>
       <c r="D4" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E4" s="22">
         <v>300</v>
@@ -1292,10 +1304,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -1307,7 +1319,7 @@
       </c>
       <c r="D5" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E5" s="4">
         <v>400</v>
@@ -1340,10 +1352,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1">
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -1355,7 +1367,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E6" s="4">
         <v>500</v>
@@ -1388,14 +1400,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1">
+    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B7" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>Mapping!D$14</f>
@@ -1403,7 +1415,7 @@
       </c>
       <c r="D7" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E7" s="4">
         <v>600</v>
@@ -1436,10 +1448,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B8" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -1484,10 +1496,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B9" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -1532,14 +1544,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B10" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C10" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -1580,10 +1592,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1">
+    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B11" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -1628,10 +1640,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1">
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B12" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -1676,14 +1688,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B13" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C13" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -1724,10 +1736,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1">
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B14" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -1772,10 +1784,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="27" customFormat="1">
+    <row r="15" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B15" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -1820,14 +1832,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1">
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B16" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -1868,10 +1880,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="1" customFormat="1">
+    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B17" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -1916,10 +1928,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B18" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -1964,14 +1976,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B19" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C19" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -2012,10 +2024,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1">
+    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B20" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -2027,7 +2039,7 @@
       </c>
       <c r="D20" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E20" s="4">
         <v>1900</v>
@@ -2060,10 +2072,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1">
+    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B21" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -2075,7 +2087,7 @@
       </c>
       <c r="D21" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E21" s="4">
         <v>2000</v>
@@ -2108,14 +2120,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1">
+    <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B22" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -2123,7 +2135,7 @@
       </c>
       <c r="D22" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E22" s="4">
         <v>2100</v>
@@ -2156,10 +2168,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="1" customFormat="1">
+    <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B23" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -2171,7 +2183,7 @@
       </c>
       <c r="D23" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E23" s="4">
         <v>2200</v>
@@ -2204,10 +2216,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="1" customFormat="1">
+    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B24" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -2219,7 +2231,7 @@
       </c>
       <c r="D24" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E24" s="4">
         <v>2300</v>
@@ -2252,14 +2264,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="27" customFormat="1">
+    <row r="25" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="str">
         <f>Mapping!D$3</f>
-        <v>1 - Harmloest</v>
+        <v>1 - Harmløst (sluff)</v>
       </c>
       <c r="B25" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C25" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -2267,7 +2279,7 @@
       </c>
       <c r="D25" s="21" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E25" s="26">
         <v>2400</v>
@@ -2300,10 +2312,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B26" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -2315,7 +2327,7 @@
       </c>
       <c r="D26" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E26" s="22">
         <v>100</v>
@@ -2348,10 +2360,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B27" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -2363,7 +2375,7 @@
       </c>
       <c r="D27" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E27" s="22">
         <v>200</v>
@@ -2396,14 +2408,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B28" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C28" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -2411,7 +2423,7 @@
       </c>
       <c r="D28" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E28" s="22">
         <v>300</v>
@@ -2444,10 +2456,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="1" customFormat="1">
+    <row r="29" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B29" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -2459,7 +2471,7 @@
       </c>
       <c r="D29" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E29" s="4">
         <v>400</v>
@@ -2492,10 +2504,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="1" customFormat="1">
+    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B30" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -2507,7 +2519,7 @@
       </c>
       <c r="D30" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E30" s="4">
         <v>500</v>
@@ -2540,14 +2552,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="1" customFormat="1">
+    <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B31" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C31" s="3" t="str">
         <f>Mapping!D$14</f>
@@ -2555,7 +2567,7 @@
       </c>
       <c r="D31" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E31" s="4">
         <v>600</v>
@@ -2588,10 +2600,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B32" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -2636,10 +2648,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B33" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -2684,14 +2696,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B34" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C34" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -2732,10 +2744,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="1" customFormat="1">
+    <row r="35" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B35" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -2780,10 +2792,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="1" customFormat="1">
+    <row r="36" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B36" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -2828,14 +2840,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B37" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C37" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -2876,10 +2888,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="1" customFormat="1">
+    <row r="38" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B38" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -2924,10 +2936,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="27" customFormat="1">
+    <row r="39" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B39" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -2972,14 +2984,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="1" customFormat="1">
+    <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B40" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C40" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -3020,10 +3032,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="1" customFormat="1">
+    <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B41" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -3068,10 +3080,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B42" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -3116,14 +3128,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B43" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C43" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -3164,10 +3176,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="1" customFormat="1">
+    <row r="44" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B44" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -3179,7 +3191,7 @@
       </c>
       <c r="D44" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E44" s="4">
         <v>1900</v>
@@ -3212,10 +3224,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="1" customFormat="1">
+    <row r="45" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B45" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -3227,7 +3239,7 @@
       </c>
       <c r="D45" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E45" s="4">
         <v>2000</v>
@@ -3260,14 +3272,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="1" customFormat="1">
+    <row r="46" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B46" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C46" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -3275,7 +3287,7 @@
       </c>
       <c r="D46" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E46" s="4">
         <v>2100</v>
@@ -3308,10 +3320,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="1" customFormat="1">
+    <row r="47" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B47" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -3323,7 +3335,7 @@
       </c>
       <c r="D47" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E47" s="4">
         <v>2200</v>
@@ -3356,10 +3368,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="1" customFormat="1">
+    <row r="48" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B48" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -3371,7 +3383,7 @@
       </c>
       <c r="D48" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E48" s="4">
         <v>2300</v>
@@ -3404,14 +3416,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="27" customFormat="1">
+    <row r="49" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="str">
         <f>Mapping!D$4</f>
-        <v>2 - Smaa</v>
+        <v>2 - Små</v>
       </c>
       <c r="B49" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C49" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -3419,7 +3431,7 @@
       </c>
       <c r="D49" s="21" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E49" s="26">
         <v>2400</v>
@@ -3452,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3467,7 +3479,7 @@
       </c>
       <c r="D50" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E50" s="22">
         <v>100</v>
@@ -3500,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3515,7 +3527,7 @@
       </c>
       <c r="D51" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E51" s="22">
         <v>200</v>
@@ -3548,14 +3560,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B52" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C52" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -3563,7 +3575,7 @@
       </c>
       <c r="D52" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E52" s="22">
         <v>300</v>
@@ -3596,7 +3608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="1" customFormat="1">
+    <row r="53" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3611,7 +3623,7 @@
       </c>
       <c r="D53" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E53" s="4">
         <v>400</v>
@@ -3644,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="1" customFormat="1">
+    <row r="54" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3659,7 +3671,7 @@
       </c>
       <c r="D54" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E54" s="4">
         <v>500</v>
@@ -3692,14 +3704,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="1" customFormat="1">
+    <row r="55" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B55" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C55" s="3" t="str">
         <f>Mapping!D$14</f>
@@ -3707,7 +3719,7 @@
       </c>
       <c r="D55" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E55" s="4">
         <v>600</v>
@@ -3740,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3788,7 +3800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3836,14 +3848,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B58" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C58" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -3884,7 +3896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="1" customFormat="1">
+    <row r="59" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3932,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="1" customFormat="1">
+    <row r="60" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -3980,14 +3992,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B61" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C61" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -4028,7 +4040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="1" customFormat="1">
+    <row r="62" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4076,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="27" customFormat="1">
+    <row r="63" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4124,14 +4136,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="1" customFormat="1">
+    <row r="64" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B64" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C64" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -4172,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="1" customFormat="1">
+    <row r="65" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4220,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4268,14 +4280,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B67" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C67" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -4316,7 +4328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="1" customFormat="1">
+    <row r="68" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4331,7 +4343,7 @@
       </c>
       <c r="D68" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E68" s="4">
         <v>1900</v>
@@ -4364,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="1" customFormat="1">
+    <row r="69" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4379,7 +4391,7 @@
       </c>
       <c r="D69" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E69" s="4">
         <v>2000</v>
@@ -4412,14 +4424,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="1" customFormat="1">
+    <row r="70" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B70" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C70" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -4427,7 +4439,7 @@
       </c>
       <c r="D70" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E70" s="4">
         <v>2100</v>
@@ -4460,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="1" customFormat="1">
+    <row r="71" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4475,7 +4487,7 @@
       </c>
       <c r="D71" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E71" s="4">
         <v>2200</v>
@@ -4508,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="1" customFormat="1">
+    <row r="72" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
@@ -4523,7 +4535,7 @@
       </c>
       <c r="D72" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E72" s="4">
         <v>2300</v>
@@ -4556,14 +4568,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="27" customFormat="1">
+    <row r="73" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="21" t="str">
         <f>Mapping!D$5</f>
         <v>3 - Middels</v>
       </c>
       <c r="B73" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C73" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -4571,7 +4583,7 @@
       </c>
       <c r="D73" s="21" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E73" s="26">
         <v>2400</v>
@@ -4604,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4619,7 +4631,7 @@
       </c>
       <c r="D74" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E74" s="22">
         <v>100</v>
@@ -4652,7 +4664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4667,7 +4679,7 @@
       </c>
       <c r="D75" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E75" s="22">
         <v>200</v>
@@ -4700,14 +4712,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B76" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C76" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -4715,7 +4727,7 @@
       </c>
       <c r="D76" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E76" s="22">
         <v>300</v>
@@ -4748,7 +4760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="1" customFormat="1">
+    <row r="77" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4763,7 +4775,7 @@
       </c>
       <c r="D77" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E77" s="4">
         <v>400</v>
@@ -4796,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" s="1" customFormat="1">
+    <row r="78" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4811,7 +4823,7 @@
       </c>
       <c r="D78" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E78" s="4">
         <v>500</v>
@@ -4844,14 +4856,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="1" customFormat="1">
+    <row r="79" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B79" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C79" s="3" t="str">
         <f>Mapping!D$14</f>
@@ -4859,7 +4871,7 @@
       </c>
       <c r="D79" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E79" s="4">
         <v>600</v>
@@ -4892,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4940,7 +4952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -4988,14 +5000,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B82" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C82" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -5036,7 +5048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="1" customFormat="1">
+    <row r="83" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5084,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="1" customFormat="1">
+    <row r="84" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5132,14 +5144,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B85" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C85" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -5180,7 +5192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="1" customFormat="1">
+    <row r="86" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5228,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="27" customFormat="1">
+    <row r="87" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5276,14 +5288,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="1" customFormat="1">
+    <row r="88" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B88" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C88" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -5324,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" s="1" customFormat="1">
+    <row r="89" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5372,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5420,14 +5432,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B91" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C91" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -5468,7 +5480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="1" customFormat="1">
+    <row r="92" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5483,7 +5495,7 @@
       </c>
       <c r="D92" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E92" s="4">
         <v>1900</v>
@@ -5516,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" s="1" customFormat="1">
+    <row r="93" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5531,7 +5543,7 @@
       </c>
       <c r="D93" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E93" s="4">
         <v>2000</v>
@@ -5564,14 +5576,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" s="1" customFormat="1">
+    <row r="94" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B94" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C94" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -5579,7 +5591,7 @@
       </c>
       <c r="D94" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E94" s="4">
         <v>2100</v>
@@ -5612,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" s="1" customFormat="1">
+    <row r="95" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5627,7 +5639,7 @@
       </c>
       <c r="D95" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E95" s="4">
         <v>2200</v>
@@ -5660,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" s="1" customFormat="1">
+    <row r="96" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
@@ -5675,7 +5687,7 @@
       </c>
       <c r="D96" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E96" s="4">
         <v>2300</v>
@@ -5708,14 +5720,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="27" customFormat="1">
+    <row r="97" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="str">
         <f>Mapping!D$6</f>
         <v>4 - Store</v>
       </c>
       <c r="B97" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C97" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -5723,7 +5735,7 @@
       </c>
       <c r="D97" s="21" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E97" s="26">
         <v>2400</v>
@@ -5756,10 +5768,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B98" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -5771,7 +5783,7 @@
       </c>
       <c r="D98" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E98" s="22">
         <v>100</v>
@@ -5804,10 +5816,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B99" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -5819,7 +5831,7 @@
       </c>
       <c r="D99" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E99" s="22">
         <v>200</v>
@@ -5852,14 +5864,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B100" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C100" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -5867,7 +5879,7 @@
       </c>
       <c r="D100" s="21" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E100" s="22">
         <v>300</v>
@@ -5900,10 +5912,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" s="1" customFormat="1">
+    <row r="101" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B101" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -5915,7 +5927,7 @@
       </c>
       <c r="D101" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E101" s="4">
         <v>400</v>
@@ -5948,10 +5960,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="1" customFormat="1">
+    <row r="102" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B102" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -5963,7 +5975,7 @@
       </c>
       <c r="D102" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E102" s="4">
         <v>500</v>
@@ -5996,14 +6008,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" s="1" customFormat="1">
+    <row r="103" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B103" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C103" s="3" t="str">
         <f>Mapping!D$14</f>
@@ -6011,7 +6023,7 @@
       </c>
       <c r="D103" s="3" t="str">
         <f>Mapping!D$16</f>
-        <v>Isolerte faresoner</v>
+        <v>Få bratte heng</v>
       </c>
       <c r="E103" s="4">
         <v>600</v>
@@ -6044,10 +6056,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B104" s="21" t="str">
         <f>Mapping!D$9</f>
@@ -6092,10 +6104,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B105" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -6140,14 +6152,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B106" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C106" s="21" t="str">
         <f>Mapping!D$13</f>
@@ -6188,10 +6200,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="1" customFormat="1">
+    <row r="107" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B107" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -6236,10 +6248,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" s="1" customFormat="1">
+    <row r="108" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B108" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -6284,14 +6296,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B109" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C109" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -6332,10 +6344,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" s="1" customFormat="1">
+    <row r="110" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B110" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -6377,10 +6389,10 @@
         <v>gray</v>
       </c>
     </row>
-    <row r="111" spans="1:12" s="27" customFormat="1">
+    <row r="111" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B111" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -6425,14 +6437,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="1" customFormat="1">
+    <row r="112" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B112" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C112" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -6473,10 +6485,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" s="1" customFormat="1">
+    <row r="113" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B113" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -6521,10 +6533,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B114" s="21" t="str">
         <f>Mapping!D$10</f>
@@ -6569,14 +6581,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B115" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C115" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -6617,10 +6629,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:12" s="1" customFormat="1">
+    <row r="116" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B116" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -6632,7 +6644,7 @@
       </c>
       <c r="D116" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E116" s="4">
         <v>1900</v>
@@ -6665,10 +6677,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" s="1" customFormat="1">
+    <row r="117" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B117" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -6680,7 +6692,7 @@
       </c>
       <c r="D117" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E117" s="4">
         <v>2000</v>
@@ -6713,14 +6725,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="1" customFormat="1">
+    <row r="118" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B118" s="3" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C118" s="3" t="str">
         <f>Mapping!D$13</f>
@@ -6728,7 +6740,7 @@
       </c>
       <c r="D118" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E118" s="4">
         <v>2100</v>
@@ -6761,10 +6773,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="1" customFormat="1">
+    <row r="119" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B119" s="3" t="str">
         <f>Mapping!D$9</f>
@@ -6776,7 +6788,7 @@
       </c>
       <c r="D119" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E119" s="4">
         <v>2200</v>
@@ -6809,10 +6821,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" s="1" customFormat="1">
+    <row r="120" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B120" s="3" t="str">
         <f>Mapping!D$10</f>
@@ -6824,7 +6836,7 @@
       </c>
       <c r="D120" s="3" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E120" s="4">
         <v>2300</v>
@@ -6857,14 +6869,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" s="27" customFormat="1">
+    <row r="121" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="21" t="str">
         <f>Mapping!D$7</f>
-        <v>5 - Svaert store</v>
+        <v>5 - Svært store</v>
       </c>
       <c r="B121" s="21" t="str">
         <f>Mapping!D$11</f>
-        <v>Naturlig utloest</v>
+        <v>Naturlig utløst</v>
       </c>
       <c r="C121" s="21" t="str">
         <f>Mapping!D$14</f>
@@ -6872,7 +6884,7 @@
       </c>
       <c r="D121" s="21" t="str">
         <f>Mapping!D$19</f>
-        <v>De fleste bratte heng, Ogsaa i mindre bratt terreng</v>
+        <v>De fleste bratte heng, Også i mindre bratt terreng</v>
       </c>
       <c r="E121" s="26">
         <v>2400</v>
@@ -6908,11 +6920,6 @@
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6921,10 +6928,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
@@ -6935,109 +6942,109 @@
     <col min="7" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="18">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E3" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="E4" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E7" s="8">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -7045,42 +7052,42 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -7088,31 +7095,31 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -7120,53 +7127,53 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="B17" s="8" t="s">
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="B19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -7174,35 +7181,30 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>